<commit_message>
added login page class files and changes related to this
</commit_message>
<xml_diff>
--- a/src/test/resources/DsAlgoTestData.xlsx
+++ b/src/test/resources/DsAlgoTestData.xlsx
@@ -8,16 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uvaraj/eclipse-workspace/CucumberBdd/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFD25A3-B46D-6A42-A324-98D73FBFFB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5B72EF-F0E1-2C41-8F89-5007644CCABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="oL3RjcO/4ojlaAIh9grc/kxGDgPAIuSvWE9GMOkS3iQ="/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>TestCase</t>
   </si>
@@ -258,12 +269,27 @@
   <si>
     <t>EmptyUsername</t>
   </si>
+  <si>
+    <t xml:space="preserve">EmptyFields </t>
+  </si>
+  <si>
+    <t>InvalidUsername</t>
+  </si>
+  <si>
+    <t>ValidDetails</t>
+  </si>
+  <si>
+    <t>co#$$%</t>
+  </si>
+  <si>
+    <t>ExpectedMesg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -316,6 +342,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -400,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -426,6 +465,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -873,7 +914,7 @@
       <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="5"/>
@@ -910,7 +951,7 @@
       <c r="F7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -945,7 +986,7 @@
       <c r="F8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -980,7 +1021,7 @@
       <c r="F9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="5" t="s">
         <v>34</v>
       </c>
@@ -29755,7 +29796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD73AE4F-5D75-C646-B7D1-12D8BD4AB874}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -29795,10 +29836,10 @@
       <c r="B2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -29849,7 +29890,7 @@
       <c r="B5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" t="s">
         <v>41</v>
       </c>
       <c r="E5" t="s">
@@ -29926,10 +29967,10 @@
       <c r="B9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -29942,4 +29983,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9241AD-8825-0F4A-8C08-6E9FFB096576}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes for cross browsing test
</commit_message>
<xml_diff>
--- a/src/test/resources/DsAlgoTestData.xlsx
+++ b/src/test/resources/DsAlgoTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uvaraj/eclipse-workspace/CucumberBdd/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5B72EF-F0E1-2C41-8F89-5007644CCABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3AF080-7D69-1A49-B6FB-2D3E9C92ADC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
     <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="DataStructures" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>TestCase</t>
   </si>
@@ -284,6 +285,18 @@
   <si>
     <t>ExpectedMesg</t>
   </si>
+  <si>
+    <t>InvalidCode</t>
+  </si>
+  <si>
+    <t>ValidCode</t>
+  </si>
+  <si>
+    <t>print("this is valid");</t>
+  </si>
+  <si>
+    <t>this is valid</t>
+  </si>
 </sst>
 </file>
 
@@ -439,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -472,7 +485,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -29989,8 +30001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9241AD-8825-0F4A-8C08-6E9FFB096576}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -30055,7 +30067,7 @@
       <c r="B6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -30065,4 +30077,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E5C803-4173-AC4B-BD58-CA617BEDED18}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B4" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>